<commit_message>
i hate microsoft graph api
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/familienbudget.xlsx
+++ b/app/src/main/res/raw/familienbudget.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A95BCD-140B-48E6-B2CE-E3C10E6C9E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F62178-993B-45E3-90EB-C5B35D3A5A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="2985" windowWidth="24720" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="12" r:id="rId1"/>
@@ -1805,7 +1805,7 @@
   <dxfs count="107">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1815,277 +1815,57 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
         <color theme="0" tint="-0.34998626667073579"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2346,31 +2126,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2381,9 +2136,6 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
@@ -2401,9 +2153,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2418,9 +2167,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2432,9 +2178,6 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
@@ -2453,9 +2196,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2471,9 +2211,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2489,9 +2226,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2507,9 +2241,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2525,9 +2256,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2543,9 +2271,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2561,9 +2286,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2576,9 +2298,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
@@ -2604,7 +2323,41 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
       <font>
@@ -2631,26 +2384,22 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="2"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2677,26 +2426,22 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="2"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2723,26 +2468,22 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="2"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2769,26 +2510,22 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="2"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2815,26 +2552,22 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="2"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2861,26 +2594,22 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="2"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2904,6 +2633,277 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="2"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="2"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="2"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="2"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="2"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="2"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -6434,47 +6434,47 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{E8724A05-F646-9544-B2FF-848649D6CB60}" name="tblVerfügbaresBarvermögen16719202329" displayName="tblVerfügbaresBarvermögen16719202329" ref="B4:P6" totalsRowCount="1">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{0AE39526-B3FC-6640-8225-AF3730203D42}" name="VERFÜGBARES BARVERMÖGEN" totalsRowLabel="Total" dataDxfId="83" totalsRowDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{C95D733F-A3E4-8547-87A4-90FB85C41E8F}" name="JAN" dataDxfId="82" totalsRowDxfId="13" dataCellStyle="20 % - Akzent1">
+    <tableColumn id="1" xr3:uid="{0AE39526-B3FC-6640-8225-AF3730203D42}" name="VERFÜGBARES BARVERMÖGEN" totalsRowLabel="Total" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{C95D733F-A3E4-8547-87A4-90FB85C41E8F}" name="JAN" dataDxfId="81" totalsRowDxfId="80" dataCellStyle="20 % - Akzent1">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[JAN]]-tblAusgaben15618222531[[#Totals],[JAN]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6EDFECA3-B0D9-B64D-8802-6D1BDD7B76D3}" name="FEB" dataDxfId="81" totalsRowDxfId="12" dataCellStyle="20 % - Akzent1">
+    <tableColumn id="3" xr3:uid="{6EDFECA3-B0D9-B64D-8802-6D1BDD7B76D3}" name="FEB" dataDxfId="79" totalsRowDxfId="78" dataCellStyle="20 % - Akzent1">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[FEB]]-tblAusgaben15618222531[[#Totals],[FEB]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8B6E8721-FFE7-9744-ACA2-FAADBE96EB8D}" name="MÄR" dataDxfId="80" totalsRowDxfId="11">
+    <tableColumn id="4" xr3:uid="{8B6E8721-FFE7-9744-ACA2-FAADBE96EB8D}" name="MÄR" dataDxfId="77" totalsRowDxfId="76">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[MÄR]]-tblAusgaben15618222531[[#Totals],[MÄR]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{DF3D0AC4-F3E1-514F-AC87-6FB6D84F6D1B}" name="APR" dataDxfId="79" totalsRowDxfId="10">
+    <tableColumn id="5" xr3:uid="{DF3D0AC4-F3E1-514F-AC87-6FB6D84F6D1B}" name="APR" dataDxfId="75" totalsRowDxfId="74">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[APR]]-tblAusgaben15618222531[[#Totals],[APR]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{29F270C9-C02B-7245-83D2-B019A3A75C37}" name="MAI" dataDxfId="78" totalsRowDxfId="9" dataCellStyle="20 % - Akzent1">
+    <tableColumn id="6" xr3:uid="{29F270C9-C02B-7245-83D2-B019A3A75C37}" name="MAI" dataDxfId="73" totalsRowDxfId="72" dataCellStyle="20 % - Akzent1">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[MAI]]-tblAusgaben15618222531[[#Totals],[MAI]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD603499-7ABD-E34C-B4AC-3CB09CB5AC23}" name="JUN" dataDxfId="77" totalsRowDxfId="8">
+    <tableColumn id="7" xr3:uid="{FD603499-7ABD-E34C-B4AC-3CB09CB5AC23}" name="JUN" dataDxfId="71" totalsRowDxfId="70">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[JUN]]-tblAusgaben15618222531[[#Totals],[JUN]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{3229E0E4-3131-F649-B857-0CD9E70221BB}" name="JUL" dataDxfId="76" totalsRowDxfId="7">
+    <tableColumn id="8" xr3:uid="{3229E0E4-3131-F649-B857-0CD9E70221BB}" name="JUL" dataDxfId="69" totalsRowDxfId="68">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[JUL]]-tblAusgaben15618222531[[#Totals],[JUL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1E417B19-7950-7148-AB0E-3BF69A91E900}" name="AUG" dataDxfId="75" totalsRowDxfId="6">
+    <tableColumn id="9" xr3:uid="{1E417B19-7950-7148-AB0E-3BF69A91E900}" name="AUG" dataDxfId="67" totalsRowDxfId="66">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[AUG]]-tblAusgaben15618222531[[#Totals],[AUG]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{96CD599A-4B63-B44B-9744-A4E5DAA82BEC}" name="SEP" dataDxfId="74" totalsRowDxfId="5">
+    <tableColumn id="10" xr3:uid="{96CD599A-4B63-B44B-9744-A4E5DAA82BEC}" name="SEP" dataDxfId="65" totalsRowDxfId="64">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[SEP]]-tblAusgaben15618222531[[#Totals],[SEP]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{6B2FBF4C-BB08-934C-B40C-268D0B7F79B6}" name="OKT" dataDxfId="73" totalsRowDxfId="4" dataCellStyle="20 % - Akzent1">
+    <tableColumn id="11" xr3:uid="{6B2FBF4C-BB08-934C-B40C-268D0B7F79B6}" name="OKT" dataDxfId="63" totalsRowDxfId="62" dataCellStyle="20 % - Akzent1">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[OKT]]-tblAusgaben15618222531[[#Totals],[OKT]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{10EFC6F3-D779-3D46-A33A-082023F36C6C}" name="NOV" dataDxfId="72" totalsRowDxfId="3">
+    <tableColumn id="12" xr3:uid="{10EFC6F3-D779-3D46-A33A-082023F36C6C}" name="NOV" dataDxfId="61" totalsRowDxfId="60">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[NOV]]-tblAusgaben15618222531[[#Totals],[NOV]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{1BA3156F-631B-E84E-91A2-4274A826A8C7}" name="DEZ" dataDxfId="71" totalsRowDxfId="2">
+    <tableColumn id="13" xr3:uid="{1BA3156F-631B-E84E-91A2-4274A826A8C7}" name="DEZ" dataDxfId="59" totalsRowDxfId="58">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[DEZ]]-tblAusgaben15618222531[[#Totals],[DEZ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F17B4F91-3015-074F-901F-56A273A71859}" name="SUMME JAHR 2023" dataDxfId="70" totalsRowDxfId="1">
+    <tableColumn id="14" xr3:uid="{F17B4F91-3015-074F-901F-56A273A71859}" name="SUMME JAHR 2023" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula>tblEinkünfte14517212430[[#Totals],[SUMME JAHR 2023]]-tblAusgaben15618222531[[#Totals],[SUMME JAHR 2023]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E3073816-CDB6-E649-BC60-309D7006970B}" name="TREND" totalsRowFunction="count" totalsRowDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{E3073816-CDB6-E649-BC60-309D7006970B}" name="TREND" totalsRowFunction="count" totalsRowDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="Family Budget Cash Available" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -6488,20 +6488,20 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{55F4908F-7C3C-984E-86B6-12801809028E}" name="tblEinkünfte14517212430" displayName="tblEinkünfte14517212430" ref="B7:P13" totalsRowCount="1">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{50B37A48-2A7D-B24A-8A01-13A6819254D5}" name="ART DER EINKÜNFTE" totalsRowLabel="SUMME EINKÜNFTE" totalsRowDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{3A48B31E-B573-344A-9A8F-A4878B97607F}" name="JAN" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{B7D8F764-5D71-2E49-B590-BECB528E409E}" name="FEB" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{64DA6F4D-EAB4-E942-9C1B-26D49F228991}" name="MÄR" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{25A969BE-F03F-8140-92F3-B18A97E304AB}" name="APR" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{CE539AD9-EAEB-D141-B279-7FFEF82C96DA}" name="MAI" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{D6C1F6DF-FE33-A14D-8D90-BA3AB0E597B2}" name="JUN" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{D283B267-F12F-AF44-A63C-4ADC3C76AF43}" name="JUL" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{89DB3DFA-F45B-D545-B5EA-54DF9C2F7096}" name="AUG" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{107DF012-45E6-AD43-BFDE-B2B57721DBA0}" name="SEP" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{6791ED38-2893-3048-AE1B-8F7B5351C11C}" name="OKT" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{217F611F-8DB4-AE47-A981-2B737779DA0C}" name="NOV" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="13" xr3:uid="{1653F2F7-EC69-2A43-B56A-F85AC1BF417D}" name="DEZ" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="14" xr3:uid="{CF0BCB5A-0DCE-1348-B28A-04EC541FE62A}" name="SUMME JAHR 2023" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="43">
+    <tableColumn id="1" xr3:uid="{50B37A48-2A7D-B24A-8A01-13A6819254D5}" name="ART DER EINKÜNFTE" totalsRowLabel="SUMME EINKÜNFTE" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{3A48B31E-B573-344A-9A8F-A4878B97607F}" name="JAN" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{B7D8F764-5D71-2E49-B590-BECB528E409E}" name="FEB" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{64DA6F4D-EAB4-E942-9C1B-26D49F228991}" name="MÄR" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{25A969BE-F03F-8140-92F3-B18A97E304AB}" name="APR" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{CE539AD9-EAEB-D141-B279-7FFEF82C96DA}" name="MAI" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{D6C1F6DF-FE33-A14D-8D90-BA3AB0E597B2}" name="JUN" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{D283B267-F12F-AF44-A63C-4ADC3C76AF43}" name="JUL" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{89DB3DFA-F45B-D545-B5EA-54DF9C2F7096}" name="AUG" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{107DF012-45E6-AD43-BFDE-B2B57721DBA0}" name="SEP" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{6791ED38-2893-3048-AE1B-8F7B5351C11C}" name="OKT" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{217F611F-8DB4-AE47-A981-2B737779DA0C}" name="NOV" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{1653F2F7-EC69-2A43-B56A-F85AC1BF417D}" name="DEZ" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{CF0BCB5A-0DCE-1348-B28A-04EC541FE62A}" name="SUMME JAHR 2023" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="0">
       <calculatedColumnFormula>SUM(tblEinkünfte14517212430[[#This Row],[JAN]:[DEZ]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{09B528FF-A033-EC4B-BA0D-DA2E35FEC351}" name="TREND"/>
@@ -6519,22 +6519,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{6A0B4C2D-263E-394E-AE4F-A659111F1760}" name="tblAusgaben15618222531" displayName="tblAusgaben15618222531" ref="B15:P53" totalsRowCount="1">
   <autoFilter ref="B15:P52" xr:uid="{6A0B4C2D-263E-394E-AE4F-A659111F1760}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{6CC7B4A8-CA2B-3E40-BAC9-5D615401C80C}" name="AUSGABEN" totalsRowLabel="SUMME AUSGABEN" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{A3C513FB-E2CB-7945-9485-8207701EB78F}" name="JAN" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{763EC9CF-27E1-9B4D-B734-D0DA3F0B7618}" name="FEB" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37">
+    <tableColumn id="1" xr3:uid="{6CC7B4A8-CA2B-3E40-BAC9-5D615401C80C}" name="AUSGABEN" totalsRowLabel="SUMME AUSGABEN" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{A3C513FB-E2CB-7945-9485-8207701EB78F}" name="JAN" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{763EC9CF-27E1-9B4D-B734-D0DA3F0B7618}" name="FEB" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36">
       <calculatedColumnFormula>D57</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F4561959-3B3E-7C4A-A1F2-B489B233D70D}" name="MÄR" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{4EDCAA1D-031F-214F-9C28-5F4D5E769D30}" name="APR" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{1929FBAF-BCCD-3E42-BCAB-74816812174D}" name="MAI" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{E1DB1B75-6488-1E4F-8197-820E1E2E9354}" name="JUN" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{39D19C53-276E-984B-9B81-30C0E6D5E5A5}" name="JUL" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{9DEDA9E2-4AD9-6841-921F-F63E4AA933C9}" name="AUG" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{D8AE48F4-C320-5249-A534-F95B5B56E62A}" name="SEP" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{645901E0-8162-6246-BEC5-67BBE69D1D5D}" name="OKT" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{EF19FEAB-B424-3546-A5B4-7D4C1845CA71}" name="NOV" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{8F100F73-1CFF-6142-AE1B-FB1DE83D5C9C}" name="DEZ" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{7EE11F30-D669-3F47-A3AA-25545351F2D6}" name="SUMME JAHR 2023" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15">
+    <tableColumn id="4" xr3:uid="{F4561959-3B3E-7C4A-A1F2-B489B233D70D}" name="MÄR" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{4EDCAA1D-031F-214F-9C28-5F4D5E769D30}" name="APR" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{1929FBAF-BCCD-3E42-BCAB-74816812174D}" name="MAI" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{E1DB1B75-6488-1E4F-8197-820E1E2E9354}" name="JUN" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{39D19C53-276E-984B-9B81-30C0E6D5E5A5}" name="JUL" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{9DEDA9E2-4AD9-6841-921F-F63E4AA933C9}" name="AUG" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{D8AE48F4-C320-5249-A534-F95B5B56E62A}" name="SEP" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{645901E0-8162-6246-BEC5-67BBE69D1D5D}" name="OKT" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{EF19FEAB-B424-3546-A5B4-7D4C1845CA71}" name="NOV" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{8F100F73-1CFF-6142-AE1B-FB1DE83D5C9C}" name="DEZ" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{7EE11F30-D669-3F47-A3AA-25545351F2D6}" name="SUMME JAHR 2023" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>SUM(tblAusgaben15618222531[[#This Row],[JAN]:[DEZ]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{B3C9DBD5-2D14-A14D-AED5-395C2933AAF7}" name="TREND"/>
@@ -6790,17 +6790,17 @@
   </sheetPr>
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A20" sqref="A20"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.42578125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="73" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="73" customWidth="1"/>
     <col min="4" max="5" width="12" style="73" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="73" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
@@ -10138,7 +10138,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{6BAB6C19-299B-4446-95E8-8ACA529CEAE6}">
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{9267E321-8250-CD4E-B0B4-EE1C649F6643}">
           <x14:colorSeries theme="5" tint="0.39997558519241921"/>
           <x14:colorNegative theme="0" tint="-0.499984740745262"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -10149,116 +10149,16 @@
           <x14:colorLow rgb="FFFF0000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'2023'!C33:N33</xm:f>
-              <xm:sqref>P33</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{18B4E044-E0B4-0440-902F-5FE962F8B776}">
-          <x14:colorSeries theme="5" tint="0.39997558519241921"/>
-          <x14:colorNegative theme="0" tint="-0.499984740745262"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="5"/>
-          <x14:colorFirst theme="6" tint="-0.249977111117893"/>
-          <x14:colorLast theme="6" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="5"/>
-          <x14:colorLow rgb="FFFF0000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'2023'!C28:N28</xm:f>
-              <xm:sqref>P28</xm:sqref>
+              <xm:f>'2023'!C30:N30</xm:f>
+              <xm:sqref>P30</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'2023'!C29:N29</xm:f>
-              <xm:sqref>P29</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{84BF304B-28E8-8849-8DFE-2B2272657D95}">
-          <x14:colorSeries theme="5" tint="0.39997558519241921"/>
-          <x14:colorNegative theme="0" tint="-0.499984740745262"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="5"/>
-          <x14:colorFirst theme="6" tint="-0.249977111117893"/>
-          <x14:colorLast theme="6" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="5"/>
-          <x14:colorLow rgb="FFFF0000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'2023'!C46:N46</xm:f>
-              <xm:sqref>P46</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap" markers="1" high="1" low="1" xr2:uid="{693BB3BC-C2F4-1F46-B58E-AB9EF9479897}">
-          <x14:colorSeries theme="5" tint="0.39997558519241921"/>
-          <x14:colorNegative theme="0" tint="-0.499984740745262"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="5"/>
-          <x14:colorFirst theme="6" tint="-0.249977111117893"/>
-          <x14:colorLast theme="6" tint="-0.249977111117893"/>
-          <x14:colorHigh rgb="FF92D050"/>
-          <x14:colorLow rgb="FFFF0000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'2023'!C8:N8</xm:f>
-              <xm:sqref>P8</xm:sqref>
+              <xm:f>'2023'!C31:N31</xm:f>
+              <xm:sqref>P31</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'2023'!C9:N9</xm:f>
-              <xm:sqref>P9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'2023'!C10:N10</xm:f>
-              <xm:sqref>P10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'2023'!C11:N11</xm:f>
-              <xm:sqref>P11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'2023'!C12:N12</xm:f>
-              <xm:sqref>P12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{82409BE1-E238-7649-8B1E-E9A14841BEDA}">
-          <x14:colorSeries theme="5" tint="0.39997558519241921"/>
-          <x14:colorNegative theme="0" tint="-0.499984740745262"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="5"/>
-          <x14:colorFirst theme="6" tint="-0.249977111117893"/>
-          <x14:colorLast theme="6" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="5"/>
-          <x14:colorLow rgb="FFFF0000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'2023'!C34:N34</xm:f>
-              <xm:sqref>P34</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="0" manualMin="0" type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{B8286966-C84B-DB40-8099-5C51C5F60FA9}">
-          <x14:colorSeries theme="5"/>
-          <x14:colorNegative rgb="FFFFB620"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD70077"/>
-          <x14:colorFirst rgb="FF777777"/>
-          <x14:colorLast rgb="FF359CEB"/>
-          <x14:colorHigh rgb="FFFF0000"/>
-          <x14:colorLow rgb="FF92D050"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'2023'!C53:N53</xm:f>
-              <xm:sqref>P53</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'2023'!C13:N13</xm:f>
-              <xm:sqref>P13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'2023'!C5:N5</xm:f>
-              <xm:sqref>P5</xm:sqref>
+              <xm:f>'2023'!C32:N32</xm:f>
+              <xm:sqref>P32</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -10390,7 +10290,31 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{9267E321-8250-CD4E-B0B4-EE1C649F6643}">
+        <x14:sparklineGroup manualMax="0" manualMin="0" type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{B8286966-C84B-DB40-8099-5C51C5F60FA9}">
+          <x14:colorSeries theme="5"/>
+          <x14:colorNegative rgb="FFFFB620"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD70077"/>
+          <x14:colorFirst rgb="FF777777"/>
+          <x14:colorLast rgb="FF359CEB"/>
+          <x14:colorHigh rgb="FFFF0000"/>
+          <x14:colorLow rgb="FF92D050"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'2023'!C53:N53</xm:f>
+              <xm:sqref>P53</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'2023'!C13:N13</xm:f>
+              <xm:sqref>P13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'2023'!C5:N5</xm:f>
+              <xm:sqref>P5</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{82409BE1-E238-7649-8B1E-E9A14841BEDA}">
           <x14:colorSeries theme="5" tint="0.39997558519241921"/>
           <x14:colorNegative theme="0" tint="-0.499984740745262"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -10401,16 +10325,92 @@
           <x14:colorLow rgb="FFFF0000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'2023'!C30:N30</xm:f>
-              <xm:sqref>P30</xm:sqref>
+              <xm:f>'2023'!C34:N34</xm:f>
+              <xm:sqref>P34</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap" markers="1" high="1" low="1" xr2:uid="{693BB3BC-C2F4-1F46-B58E-AB9EF9479897}">
+          <x14:colorSeries theme="5" tint="0.39997558519241921"/>
+          <x14:colorNegative theme="0" tint="-0.499984740745262"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="5"/>
+          <x14:colorFirst theme="6" tint="-0.249977111117893"/>
+          <x14:colorLast theme="6" tint="-0.249977111117893"/>
+          <x14:colorHigh rgb="FF92D050"/>
+          <x14:colorLow rgb="FFFF0000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'2023'!C8:N8</xm:f>
+              <xm:sqref>P8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'2023'!C31:N31</xm:f>
-              <xm:sqref>P31</xm:sqref>
+              <xm:f>'2023'!C9:N9</xm:f>
+              <xm:sqref>P9</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>'2023'!C32:N32</xm:f>
-              <xm:sqref>P32</xm:sqref>
+              <xm:f>'2023'!C10:N10</xm:f>
+              <xm:sqref>P10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'2023'!C11:N11</xm:f>
+              <xm:sqref>P11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'2023'!C12:N12</xm:f>
+              <xm:sqref>P12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{84BF304B-28E8-8849-8DFE-2B2272657D95}">
+          <x14:colorSeries theme="5" tint="0.39997558519241921"/>
+          <x14:colorNegative theme="0" tint="-0.499984740745262"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="5"/>
+          <x14:colorFirst theme="6" tint="-0.249977111117893"/>
+          <x14:colorLast theme="6" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="5"/>
+          <x14:colorLow rgb="FFFF0000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'2023'!C46:N46</xm:f>
+              <xm:sqref>P46</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{18B4E044-E0B4-0440-902F-5FE962F8B776}">
+          <x14:colorSeries theme="5" tint="0.39997558519241921"/>
+          <x14:colorNegative theme="0" tint="-0.499984740745262"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="5"/>
+          <x14:colorFirst theme="6" tint="-0.249977111117893"/>
+          <x14:colorLast theme="6" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="5"/>
+          <x14:colorLow rgb="FFFF0000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'2023'!C28:N28</xm:f>
+              <xm:sqref>P28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'2023'!C29:N29</xm:f>
+              <xm:sqref>P29</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" displayHidden="1" xr2:uid="{6BAB6C19-299B-4446-95E8-8ACA529CEAE6}">
+          <x14:colorSeries theme="5" tint="0.39997558519241921"/>
+          <x14:colorNegative theme="0" tint="-0.499984740745262"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="5"/>
+          <x14:colorFirst theme="6" tint="-0.249977111117893"/>
+          <x14:colorLast theme="6" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="5"/>
+          <x14:colorLow rgb="FFFF0000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'2023'!C33:N33</xm:f>
+              <xm:sqref>P33</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>